<commit_message>
add print score after game
</commit_message>
<xml_diff>
--- a/25.xlsx
+++ b/25.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -25,6 +25,9 @@
     <t>Unnamed: 0.1.1</t>
   </si>
   <si>
+    <t>Unnamed: 0.1.1.1</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
@@ -35,6 +38,9 @@
   </si>
   <si>
     <t>Sat Jan 18 18:45:37 2020</t>
+  </si>
+  <si>
+    <t>Sat Jan 18 19:17:08 2020</t>
   </si>
 </sst>
 </file>
@@ -392,13 +398,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,8 +420,11 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -425,36 +434,56 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>